<commit_message>
update official GDPR translations
</commit_message>
<xml_diff>
--- a/lang/official_GDPR_translations.xlsx
+++ b/lang/official_GDPR_translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snet/Documents/H2020 Projekte/2021/TRAPEZE/work packages/work package 4/TUB/privacy-dashboard/internal-repo/trapez-privacy-dashboard/lang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB4D1EF-FFB2-F349-B194-A418CFA2679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C2420-4CC5-3144-B65D-BF31AA4834A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F5AAD40B-F190-B24C-A5C1-AA6E07944652}"/>
   </bookViews>
@@ -572,7 +572,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -584,6 +584,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -606,15 +614,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC61F687-4242-4A48-8CD8-A913C446BAEC}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,7 +978,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1007,16 +1017,16 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1556,6 +1566,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{48EE1071-6312-9C4B-A27F-98A7AE70C3A2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add landing page translations
</commit_message>
<xml_diff>
--- a/lang/official_GDPR_translations.xlsx
+++ b/lang/official_GDPR_translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snet/Documents/H2020 Projekte/2021/TRAPEZE/work packages/work package 4/TUB/privacy-dashboard/internal-repo/trapez-privacy-dashboard/lang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C2420-4CC5-3144-B65D-BF31AA4834A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9991BC-B3C7-744C-AE88-58FEA2B00F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F5AAD40B-F190-B24C-A5C1-AA6E07944652}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="181">
   <si>
     <t>Glossary</t>
   </si>
@@ -566,6 +566,18 @@
   </si>
   <si>
     <t>À l'article 13, premier paragraphe, point b) RGPD</t>
+  </si>
+  <si>
+    <t>withdraw consent</t>
+  </si>
+  <si>
+    <t>Einwilligung wiederrufen</t>
+  </si>
+  <si>
+    <t>retirer consentement</t>
+  </si>
+  <si>
+    <t>ritirare consenso</t>
   </si>
 </sst>
 </file>
@@ -937,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC61F687-4242-4A48-8CD8-A913C446BAEC}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,6 +1577,20 @@
         <v>155</v>
       </c>
     </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" t="s">
+        <v>180</v>
+      </c>
+      <c r="F47" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{48EE1071-6312-9C4B-A27F-98A7AE70C3A2}"/>

</xml_diff>

<commit_message>
replace 'revoke' with 'withdraw'
</commit_message>
<xml_diff>
--- a/lang/official_GDPR_translations.xlsx
+++ b/lang/official_GDPR_translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snet/Documents/H2020 Projekte/2021/TRAPEZE/work packages/work package 4/TUB/privacy-dashboard/internal-repo/trapez-privacy-dashboard/lang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9991BC-B3C7-744C-AE88-58FEA2B00F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C82DF44-0A2E-5347-AA24-837077781D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F5AAD40B-F190-B24C-A5C1-AA6E07944652}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>Glossary</t>
   </si>
@@ -578,6 +578,12 @@
   </si>
   <si>
     <t>ritirare consenso</t>
+  </si>
+  <si>
+    <t>Einwilligung erteilen</t>
+  </si>
+  <si>
+    <t>give consent</t>
   </si>
 </sst>
 </file>
@@ -949,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC61F687-4242-4A48-8CD8-A913C446BAEC}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1591,6 +1597,14 @@
         <v>179</v>
       </c>
     </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{48EE1071-6312-9C4B-A27F-98A7AE70C3A2}"/>

</xml_diff>